<commit_message>
add more metrics to the radar notebook
</commit_message>
<xml_diff>
--- a/Writing/22-23/week1/content.xlsx
+++ b/Writing/22-23/week1/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashkarle/soccer-ds-stats/Writing/22-23/week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6A5487-240D-104F-BAB9-565416308A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C331200-8FB0-6742-9C5D-A1FDB5532394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" activeTab="7" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
   </bookViews>
   <sheets>
     <sheet name="0 Comms" sheetId="11" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="243">
   <si>
     <t>Key stats</t>
   </si>
@@ -908,6 +908,9 @@
   </si>
   <si>
     <t>OptaPro Analytics Forum</t>
+  </si>
+  <si>
+    <t>Going paid!!!</t>
   </si>
 </sst>
 </file>
@@ -1222,6 +1225,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>193249</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>112708</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7A301C9-A748-734A-B6CD-4D5CBDC4ADDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6797249" y="1449916"/>
+          <a:ext cx="8999959" cy="4370917"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1519,15 +1571,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5068ED-902C-3546-B15E-0748BE44D916}">
-  <dimension ref="B4:F20"/>
+  <dimension ref="B4:K19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
         <v>123</v>
       </c>
@@ -1535,7 +1587,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>122</v>
       </c>
@@ -1543,43 +1595,47 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:11">
       <c r="F6" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="K6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:11">
       <c r="B8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:11">
       <c r="B9" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="6:6">
-      <c r="F17" t="s">
+    <row r="16" spans="2:11">
+      <c r="B16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="6:6">
-      <c r="F18" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="6:6">
-      <c r="F20" s="16" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" s="16" t="s">
         <v>236</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3757,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB6674-CFF2-5841-B4C6-F22E6892C162}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sim matches notebook update
</commit_message>
<xml_diff>
--- a/Writing/22-23/week1/content.xlsx
+++ b/Writing/22-23/week1/content.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashkarle/soccer-ds-stats/Writing/22-23/week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B6F757-AB4D-F649-AC67-D551A6D2CA5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E439E1-1751-7D4A-AA90-649B8A2B91F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" activeTab="7" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
   </bookViews>
   <sheets>
     <sheet name="0 Comms" sheetId="11" r:id="rId1"/>
@@ -1482,6 +1482,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>52916</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>70055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>74083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19069CC0-3768-E744-8EBB-4CEC932A31F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7482416" y="5700388"/>
+          <a:ext cx="3661834" cy="3221362"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1784,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5068ED-902C-3546-B15E-0748BE44D916}">
   <dimension ref="B4:K19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -4024,7 +4068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AB6674-CFF2-5841-B4C6-F22E6892C162}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>

</xml_diff>